<commit_message>
Updated members data and cleaned up temporary files
</commit_message>
<xml_diff>
--- a/SnakeChaosHouse Members.xlsx
+++ b/SnakeChaosHouse Members.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yusfr\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\S.C.H\System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{158DA84D-4F64-4811-9841-7FC63CB437DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A629764-E8C8-4BB8-85E2-0EAFEF0BF8FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{A6127CEC-2AF5-41AD-ABBE-ED558C1027AE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="322">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -831,6 +831,177 @@
   </si>
   <si>
     <t>+20 102 346 2890</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>D85mk4Kh</t>
+  </si>
+  <si>
+    <t>CdmYUljS</t>
+  </si>
+  <si>
+    <t>FtXawwUW</t>
+  </si>
+  <si>
+    <t>AkiI7rOW</t>
+  </si>
+  <si>
+    <t>mVbMC7n2</t>
+  </si>
+  <si>
+    <t>tPypM1Ne</t>
+  </si>
+  <si>
+    <t>BSJVo8jd</t>
+  </si>
+  <si>
+    <t>DEIoeIfu</t>
+  </si>
+  <si>
+    <t>qI2pgPyk</t>
+  </si>
+  <si>
+    <t>DUMfHEKG</t>
+  </si>
+  <si>
+    <t>zoqJPTKD</t>
+  </si>
+  <si>
+    <t>5EYMDOFM</t>
+  </si>
+  <si>
+    <t>HLqiCHBU</t>
+  </si>
+  <si>
+    <t>sqm5xGG8</t>
+  </si>
+  <si>
+    <t>YHNvgkDg</t>
+  </si>
+  <si>
+    <t>UFNfsLp4</t>
+  </si>
+  <si>
+    <t>O8v66rwM</t>
+  </si>
+  <si>
+    <t>yrSfSCq7</t>
+  </si>
+  <si>
+    <t>LRRjkObr</t>
+  </si>
+  <si>
+    <t>Y7BMTHUN</t>
+  </si>
+  <si>
+    <t>aiKJySsa</t>
+  </si>
+  <si>
+    <t>aj4LoLfL</t>
+  </si>
+  <si>
+    <t>h85MBOW5</t>
+  </si>
+  <si>
+    <t>mTdNscvN</t>
+  </si>
+  <si>
+    <t>j3ya7T5o</t>
+  </si>
+  <si>
+    <t>YqGrdV0T</t>
+  </si>
+  <si>
+    <t>DoNKpVL5</t>
+  </si>
+  <si>
+    <t>NfLz5umL</t>
+  </si>
+  <si>
+    <t>Zrv5gpgj</t>
+  </si>
+  <si>
+    <t>sTWiKbV7</t>
+  </si>
+  <si>
+    <t>s1d1uTLw</t>
+  </si>
+  <si>
+    <t>xH30UiQ5</t>
+  </si>
+  <si>
+    <t>124k6x3A</t>
+  </si>
+  <si>
+    <t>pBs9E69D</t>
+  </si>
+  <si>
+    <t>7G4PLLOt</t>
+  </si>
+  <si>
+    <t>AKddEp87</t>
+  </si>
+  <si>
+    <t>m4gKPwGG</t>
+  </si>
+  <si>
+    <t>Zze6WFWe</t>
+  </si>
+  <si>
+    <t>QxKLma6O</t>
+  </si>
+  <si>
+    <t>J4LH3d7N</t>
+  </si>
+  <si>
+    <t>hHjirkz8</t>
+  </si>
+  <si>
+    <t>Jz1XKzPO</t>
+  </si>
+  <si>
+    <t>YxCI3niz</t>
+  </si>
+  <si>
+    <t>CO9dP7Ts</t>
+  </si>
+  <si>
+    <t>JwswhoBU</t>
+  </si>
+  <si>
+    <t>vGidvj1X</t>
+  </si>
+  <si>
+    <t>XIU89l07</t>
+  </si>
+  <si>
+    <t>akKd9Wt6</t>
+  </si>
+  <si>
+    <t>jvKwjwrF</t>
+  </si>
+  <si>
+    <t>SdPYZlg7</t>
+  </si>
+  <si>
+    <t>x9b6YYG1</t>
+  </si>
+  <si>
+    <t>BDiwelI7</t>
+  </si>
+  <si>
+    <t>pf5IhhH4</t>
+  </si>
+  <si>
+    <t>7c9ZJ5CZ</t>
+  </si>
+  <si>
+    <t>FmvCMhWX</t>
+  </si>
+  <si>
+    <t>wxgkdl8v</t>
   </si>
 </sst>
 </file>
@@ -841,7 +1012,7 @@
     <numFmt numFmtId="164" formatCode="\+00\ 000\ 000\ 0000"/>
     <numFmt numFmtId="165" formatCode="\+000\ 00\ 000\ 0000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -874,6 +1045,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -883,7 +1062,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -891,12 +1070,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -922,6 +1116,9 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1265,8 +1462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2072C2A-C789-4105-96E6-B4293345B381}">
   <dimension ref="A1:R66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="D14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1286,6 +1483,7 @@
     <col min="14" max="14" width="175.7109375" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="44" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="17.140625" customWidth="1"/>
+    <col min="18" max="18" width="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -1340,7 +1538,9 @@
       <c r="Q1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="4"/>
+      <c r="R1" s="10" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -1392,7 +1592,9 @@
       <c r="Q2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="R2" s="4"/>
+      <c r="R2" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -1444,7 +1646,9 @@
       <c r="Q3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="R3" s="4"/>
+      <c r="R3" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -1496,7 +1700,9 @@
       <c r="Q4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="R4" s="4"/>
+      <c r="R4" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -1548,7 +1754,9 @@
       <c r="Q5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="R5" s="4"/>
+      <c r="R5" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -1600,7 +1808,9 @@
       <c r="Q6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="R6" s="4"/>
+      <c r="R6" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -1650,7 +1860,9 @@
       <c r="Q7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="R7" s="4"/>
+      <c r="R7" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -1702,7 +1914,9 @@
       <c r="Q8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="R8" s="4"/>
+      <c r="R8" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -1750,7 +1964,9 @@
       <c r="Q9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="R9" s="4"/>
+      <c r="R9" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -1802,7 +2018,9 @@
       <c r="Q10" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="R10" s="4"/>
+      <c r="R10" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -1850,7 +2068,9 @@
       <c r="Q11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="R11" s="4"/>
+      <c r="R11" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -1902,7 +2122,9 @@
       <c r="Q12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="R12" s="4"/>
+      <c r="R12" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
@@ -1954,7 +2176,9 @@
       <c r="Q13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="R13" s="4"/>
+      <c r="R13" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
@@ -2006,9 +2230,11 @@
       <c r="Q14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="R14" s="4"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R14" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>72</v>
       </c>
@@ -2058,8 +2284,11 @@
       <c r="Q18" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R18" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>248</v>
       </c>
@@ -2105,8 +2334,11 @@
       <c r="Q19" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R19" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>223</v>
       </c>
@@ -2156,8 +2388,11 @@
       <c r="Q20" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R20" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>94</v>
       </c>
@@ -2207,8 +2442,11 @@
       <c r="Q21" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R21" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>79</v>
       </c>
@@ -2258,8 +2496,11 @@
       <c r="Q22" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R22" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>99</v>
       </c>
@@ -2309,8 +2550,11 @@
       <c r="Q23" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R23" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>262</v>
       </c>
@@ -2352,8 +2596,11 @@
       <c r="Q27" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R27" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>111</v>
       </c>
@@ -2399,8 +2646,11 @@
       <c r="Q28" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R28" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>117</v>
       </c>
@@ -2444,8 +2694,11 @@
       <c r="Q29" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R29" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>121</v>
       </c>
@@ -2491,8 +2744,11 @@
       <c r="Q30" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R30" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>124</v>
       </c>
@@ -2538,8 +2794,11 @@
       <c r="Q31" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R31" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>261</v>
       </c>
@@ -2581,6 +2840,9 @@
       <c r="Q32" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="R32" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
@@ -2628,6 +2890,9 @@
       <c r="Q33" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="R33" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
@@ -2674,6 +2939,9 @@
       </c>
       <c r="Q34" s="4" t="s">
         <v>23</v>
+      </c>
+      <c r="R34" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
@@ -2722,6 +2990,9 @@
       <c r="Q35" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="R35" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
@@ -2768,6 +3039,9 @@
       </c>
       <c r="Q36" s="4" t="s">
         <v>23</v>
+      </c>
+      <c r="R36" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -2816,6 +3090,9 @@
       <c r="Q37" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="R37" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
@@ -2863,6 +3140,9 @@
       <c r="Q38" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="R38" t="s">
+        <v>296</v>
+      </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
@@ -2908,6 +3188,9 @@
       <c r="Q39" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="R39" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
@@ -2955,6 +3238,9 @@
       <c r="Q40" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="R40" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
@@ -3002,6 +3288,9 @@
       <c r="Q41" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="R41" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
@@ -3046,6 +3335,9 @@
       </c>
       <c r="Q42" s="4" t="s">
         <v>23</v>
+      </c>
+      <c r="R42" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
@@ -3094,6 +3386,9 @@
       <c r="Q43" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="R43" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
@@ -3141,7 +3436,9 @@
       <c r="Q44" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="R44" s="4"/>
+      <c r="R44" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
@@ -3186,6 +3483,9 @@
       </c>
       <c r="Q45" s="4" t="s">
         <v>23</v>
+      </c>
+      <c r="R45" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
@@ -3207,7 +3507,7 @@
       <c r="P48" s="4"/>
       <c r="Q48" s="4"/>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>164</v>
       </c>
@@ -3253,8 +3553,11 @@
       <c r="Q49" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R49" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>168</v>
       </c>
@@ -3300,8 +3603,11 @@
       <c r="Q50" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R50" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>171</v>
       </c>
@@ -3345,8 +3651,11 @@
       <c r="Q51" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R51" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>173</v>
       </c>
@@ -3392,8 +3701,11 @@
       <c r="Q52" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R52" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>178</v>
       </c>
@@ -3439,8 +3751,11 @@
       <c r="Q53" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R53" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>182</v>
       </c>
@@ -3486,8 +3801,11 @@
       <c r="Q54" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R54" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>186</v>
       </c>
@@ -3533,8 +3851,11 @@
       <c r="Q55" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R55" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>190</v>
       </c>
@@ -3580,8 +3901,11 @@
       <c r="Q56" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R56" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>193</v>
       </c>
@@ -3627,8 +3951,11 @@
       <c r="Q57" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R57" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>198</v>
       </c>
@@ -3674,8 +4001,11 @@
       <c r="Q58" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R58" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>200</v>
       </c>
@@ -3721,8 +4051,11 @@
       <c r="Q59" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R59" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>204</v>
       </c>
@@ -3768,8 +4101,11 @@
       <c r="Q60" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R60" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>207</v>
       </c>
@@ -3815,8 +4151,11 @@
       <c r="Q61" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R61" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>212</v>
       </c>
@@ -3862,8 +4201,11 @@
       <c r="Q62" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R62" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>216</v>
       </c>
@@ -3909,8 +4251,11 @@
       <c r="Q63" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R63" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>233</v>
       </c>
@@ -3956,8 +4301,11 @@
       <c r="Q64" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R64" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>219</v>
       </c>
@@ -4003,8 +4351,11 @@
       <c r="Q65" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R65" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>242</v>
       </c>
@@ -4049,6 +4400,9 @@
       </c>
       <c r="Q66" s="4" t="s">
         <v>23</v>
+      </c>
+      <c r="R66" t="s">
+        <v>321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>